<commit_message>
Added table for all lenders to calc % total jumbo.
</commit_message>
<xml_diff>
--- a/Jumbo/cleanedData/JumboByYear.xlsx
+++ b/Jumbo/cleanedData/JumboByYear.xlsx
@@ -5,22 +5,36 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hwpubs-my.sharepoint.com/personal/will_hwmedia_com/Documents/Documents/Coding/HMDA/cleanedData/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hwpubs-my.sharepoint.com/personal/will_hwmedia_com/Documents/Documents/Coding/HMDA/Jumbo/cleanedData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="11_08B5054C1B72FEAEE46394D757245E3FB48F8985" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B33CD960-1ED8-41ED-B98A-AE832DB96BDD}"/>
+  <xr:revisionPtr revIDLastSave="17" documentId="11_08B5054C1B72FEAEE46394D757245E3FB48F8985" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C5282849-6C3E-43BF-9D39-8D96EE9440C8}"/>
   <bookViews>
-    <workbookView xWindow="41400" yWindow="510" windowWidth="19200" windowHeight="11175" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="JumboData" sheetId="1" r:id="rId1"/>
+    <sheet name="allLendersByYear" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Year</t>
   </si>
@@ -41,16 +55,24 @@
   </si>
   <si>
     <t>% Loans Jumbo</t>
+  </si>
+  <si>
+    <t>activity_year</t>
+  </si>
+  <si>
+    <t>lenders</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="3">
     <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="166" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -62,6 +84,13 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -96,10 +125,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -107,8 +137,11 @@
     <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -122,6 +155,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -412,7 +449,7 @@
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="M13" sqref="M13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -459,14 +496,15 @@
       <c r="C2" s="3">
         <v>336593</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="5">
         <v>4026</v>
       </c>
       <c r="E2" s="4">
         <v>0.24379999999999999</v>
       </c>
       <c r="F2" s="4">
-        <v>0.42359999999999998</v>
+        <f>D2/allLendersByYear!B2</f>
+        <v>0.73426956045960246</v>
       </c>
       <c r="G2" s="4">
         <v>0.08</v>
@@ -482,14 +520,15 @@
       <c r="C3" s="3">
         <v>423993</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="5">
         <v>3947</v>
       </c>
       <c r="E3" s="4">
         <v>0.2364</v>
       </c>
       <c r="F3" s="4">
-        <v>0.4244</v>
+        <f>D3/allLendersByYear!B3</f>
+        <v>0.73665546845838004</v>
       </c>
       <c r="G3" s="4">
         <v>7.8899999999999998E-2</v>
@@ -505,14 +544,15 @@
       <c r="C4" s="3">
         <v>527980</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="5">
         <v>3549</v>
       </c>
       <c r="E4" s="4">
         <v>0.15759999999999999</v>
       </c>
       <c r="F4" s="4">
-        <v>0.44890000000000002</v>
+        <f>D4/allLendersByYear!B4</f>
+        <v>0.81417756366139027</v>
       </c>
       <c r="G4" s="4">
         <v>5.2299999999999999E-2</v>
@@ -528,14 +568,15 @@
       <c r="C5" s="3">
         <v>584605</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="5">
         <v>3260</v>
       </c>
       <c r="E5" s="4">
         <v>0.19009999999999999</v>
       </c>
       <c r="F5" s="4">
-        <v>0.436</v>
+        <f>D5/allLendersByYear!B5</f>
+        <v>0.77214590241591663</v>
       </c>
       <c r="G5" s="4">
         <v>5.6300000000000003E-2</v>
@@ -551,14 +592,15 @@
       <c r="C6" s="3">
         <v>295477</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="5">
         <v>3122</v>
       </c>
       <c r="E6" s="4">
         <v>0.22700000000000001</v>
       </c>
       <c r="F6" s="4">
-        <v>0.42009999999999997</v>
+        <f>D6/allLendersByYear!B6</f>
+        <v>0.72436194895591643</v>
       </c>
       <c r="G6" s="4">
         <v>6.4399999999999999E-2</v>
@@ -567,4 +609,72 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1382A570-F6B8-4A60-A51A-2D8A57981AB8}">
+  <dimension ref="A1:D6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="11.26953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.08984375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>2018</v>
+      </c>
+      <c r="B2" s="5">
+        <v>5483</v>
+      </c>
+      <c r="D2" s="6"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>2019</v>
+      </c>
+      <c r="B3" s="5">
+        <v>5358</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>2020</v>
+      </c>
+      <c r="B4" s="5">
+        <v>4359</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>2021</v>
+      </c>
+      <c r="B5" s="5">
+        <v>4222</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>2022</v>
+      </c>
+      <c r="B6" s="5">
+        <v>4310</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>